<commit_message>
add common excel diff
</commit_message>
<xml_diff>
--- a/test/测试分页1.xlsx
+++ b/test/测试分页1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3C026F-CF5A-4ADD-B186-D889B4172C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="555" yWindow="5100" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,8 +21,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>诉讼时效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飒飒下啊是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按顺序暗杀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗杀啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘻嘻嘻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  想啊伤心啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗杀暗杀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿斯顿撒打算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cxxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,13 +385,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B6:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -353,22 +420,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C6:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>